<commit_message>
Sorted All_results_clean by image verb then HL
</commit_message>
<xml_diff>
--- a/Behavioral testing/mturk/results/MainVerbs.xlsx
+++ b/Behavioral testing/mturk/results/MainVerbs.xlsx
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="A218" sqref="A218:A241"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A176" sqref="A2:A241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>